<commit_message>
add olympus data & general update
</commit_message>
<xml_diff>
--- a/leica_matrixscreener/08_SP8_PC/renamed_deflate/settings_channels.xlsx
+++ b/leica_matrixscreener/08_SP8_PC/renamed_deflate/settings_channels.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr date1904="false"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="1">
     <font>
@@ -472,10 +472,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
@@ -670,10 +670,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>

</xml_diff>